<commit_message>
Updated gray_Nico.xlsx with results from running gray.c on Azure
</commit_message>
<xml_diff>
--- a/blackWhite/gray_Nico.xlsx
+++ b/blackWhite/gray_Nico.xlsx
@@ -8,14 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/Mi unidad/TEC/14. AD21/Multiprocesadores/multiprocesadoresCloud/blackWhite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA962E2-BA61-C14B-AD5C-C4578880A12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADB6852-27C0-B047-8961-1EA780764BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16400" xr2:uid="{2A6433D0-8A31-F84B-B67B-09A9C8D589F6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{2A6433D0-8A31-F84B-B67B-09A9C8D589F6}"/>
   </bookViews>
   <sheets>
     <sheet name="MBP Nico" sheetId="1" r:id="rId1"/>
     <sheet name="Azure" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Azure!$A$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Azure!$A$2:$A$100</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Azure!$B$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Azure!$B$2:$B$100</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Azure!$A$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Azure!$A$2:$A$100</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Azure!$B$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Azure!$B$2:$B$100</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,12 +45,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>num_thread</t>
   </si>
   <si>
     <t>execution_time</t>
+  </si>
+  <si>
+    <t>num_threads</t>
   </si>
 </sst>
 </file>
@@ -93,6 +106,2978 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-MX"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MBP Nico'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>execution_time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MBP Nico'!$A$2:$A$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MBP Nico'!$B$2:$B$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>3.0769030000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.2826230000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1479249999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7773789999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5487789999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.2908210000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0813329999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5397619999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.3776279999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.8761900000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.3430169999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.1506059999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.2673120000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.7505280000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.8267220000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.8971150000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.7430089999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.7050020000000004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.8196479999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.875934</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.6892149999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.7348809999999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.7236919999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.6868499999999997</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.8358759999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.7373060000000002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.0382189999999998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.091107</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.8791450000000003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.7440429999999996</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.8979879999999998</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.2004640000000002</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.547625</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.38795</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.9886739999999996</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.1413710000000004</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.7984720000000003</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.4246999999999996</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.472874</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.3506130000000001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.4355760000000002</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.2030620000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.177257</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.9914839999999998</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.2260590000000002</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.3669180000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5.4395629999999997</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.871594</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.8074260000000004</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5.9611270000000003</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.1266829999999999</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.143243</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.2876570000000003</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.7789239999999999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.3224270000000002</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.3221119999999997</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.0196649999999998</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.2376399999999999</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.6912960000000004</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.8359949999999996</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.336805</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.09124</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5.5786569999999998</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.0899910000000004</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.2662959999999996</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.024686</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5.3324040000000004</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5.1633240000000002</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>5.384442</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5.600047</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>5.251404</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5.2347330000000003</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5.2932680000000003</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5.647748</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5.602036</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5.4388120000000004</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5.4368499999999997</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>5.5873619999999997</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>5.3206930000000003</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>5.1044679999999998</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>5.1707049999999999</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>5.3807260000000001</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>5.2863860000000003</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4.9911479999999999</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4.880668</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>5.1347610000000001</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>5.3235720000000004</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>5.5293570000000001</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>5.2353829999999997</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4.9672229999999997</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>4.7904689999999999</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>5.2909499999999996</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5.3678290000000004</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>5.5263939999999998</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>5.2955329999999998</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>5.0565509999999998</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>5.0440649999999998</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>5.3468879999999999</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>5.4573330000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0CF7-E04A-8889-6F25105105A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="156856048"/>
+        <c:axId val="152939648"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="156856048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="152939648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="152939648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="156856048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-MX"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Azure!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>execution_time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Azure!$A$2:$A$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Azure!$B$2:$B$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>0.37077399999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5901350000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2656209999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2153330000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.220046</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2771210000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2613340000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1482420000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.2331029999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3079689999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.2499470000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.3212190000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.315042</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.3071139999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.2469519999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.2973460000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.2396600000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.3019959999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.29196</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.3199480000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.2398910000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.2857829999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.2400090000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.2965819999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.2714500000000002</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.1589130000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.2523620000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.244205</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.2202790000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.2466659999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.240707</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.3042729999999998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.2519</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.2117010000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.0231979999999998</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.2836029999999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.251007</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.2897020000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.2773720000000002</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.2843179999999998</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.29528</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.20384</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.1930869999999998</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.2064910000000002</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.2415959999999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.313536</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.211608</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.294089</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.2713030000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3.2144550000000001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.2038500000000001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.3008549999999999</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.1355740000000001</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.2875779999999999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.2561710000000001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.2895850000000002</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.2227079999999999</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.3702200000000002</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.2358600000000002</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.2956430000000001</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.2112310000000002</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.159519</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.2701449999999999</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.2129460000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.268221</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.2969390000000001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.253463</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.1401490000000001</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.2976700000000001</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.3433299999999999</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.2240090000000001</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3.2703980000000001</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.265619</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3.3181609999999999</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.3309519999999999</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.2839469999999999</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.3283040000000002</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3.3150140000000001</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.2656130000000001</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.2344400000000002</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.2902550000000002</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.3900800000000002</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.2903009999999999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.3285999999999998</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.202512</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3.2983699999999998</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3.2696900000000002</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3.2833380000000001</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3.2509380000000001</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3.3290169999999999</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3.2719640000000001</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.3445119999999999</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3.315537</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3.2726329999999999</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.30091</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3.3112360000000001</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3.2468919999999999</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3.288395</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3.2834979999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8F79-0D48-AFA5-48938ED773C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="157085520"/>
+        <c:axId val="157087168"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="157085520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="157087168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="157087168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="157085520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C5E03BC-3139-0D42-9A60-D11CC884A9B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A695043-8323-7149-9BDF-93C3775C6562}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -394,8 +3379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C556BF45-DDDD-5B49-A9B0-E46566E4D088}">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1206,17 +4191,826 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5E8B66-0232-A345-AF80-BB3C0C9C4BB6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.37077399999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2.5901350000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3.2656209999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3.2153330000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>3.220046</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3.2771210000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3.2613340000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3.1482420000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3.2331029999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>3.3079689999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>3.2499470000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>3.3212190000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>3.315042</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>3.3071139999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>3.2469519999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>3.2973460000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>3.2396600000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>3.3019959999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>3.29196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>3.3199480000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>3.2398910000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>3.2857829999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>3.2400090000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>3.2965819999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>3.2714500000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>3.1589130000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>3.2523620000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>3.244205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>3.2202790000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>3.2466659999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>3.240707</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>3.3042729999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>3.2519</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>3.2117010000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>3.0231979999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>3.2836029999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>3.251007</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>3.2897020000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>3.2773720000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>3.2843179999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>3.29528</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>3.20384</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>3.1930869999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>3.2064910000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>3.2415959999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>3.313536</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>3.211608</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>3.294089</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>3.2713030000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>3.2144550000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>3.2038500000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>3.3008549999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>3.1355740000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>3.2875779999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>3.2561710000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>3.2895850000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>3.2227079999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>3.3702200000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>3.2358600000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>3.2956430000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>3.2112310000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>3.159519</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>3.2701449999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>3.2129460000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>3.268221</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>3.2969390000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>3.253463</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>3.1401490000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>3.2976700000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>3.3433299999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>3.2240090000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>3.2703980000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>3.265619</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>3.3181609999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>3.3309519999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>3.2839469999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>3.3283040000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>3.3150140000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>3.2656130000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>3.2344400000000002</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>3.2902550000000002</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>3.3900800000000002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>3.2903009999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>3.3285999999999998</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>3.202512</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>3.2983699999999998</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>3.2696900000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>3.2833380000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>3.2509380000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>3.3290169999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>3.2719640000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>3.3445119999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>3.315537</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>3.2726329999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>3.30091</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>3.3112360000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>3.2468919999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>3.288395</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>3.2834979999999998</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added min_time value in Excel file
</commit_message>
<xml_diff>
--- a/blackWhite/gray_Nico.xlsx
+++ b/blackWhite/gray_Nico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/Mi unidad/TEC/14. AD21/Multiprocesadores/multiprocesadoresCloud/blackWhite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADB6852-27C0-B047-8961-1EA780764BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B593215-AD4A-4049-9B3C-D2230B130089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{2A6433D0-8A31-F84B-B67B-09A9C8D589F6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2A6433D0-8A31-F84B-B67B-09A9C8D589F6}"/>
   </bookViews>
   <sheets>
     <sheet name="MBP Nico" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="_xlchart.v1.6" hidden="1">Azure!$B$1</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">Azure!$B$2:$B$100</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>num_thread</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>num_threads</t>
+  </si>
+  <si>
+    <t>min_time</t>
   </si>
 </sst>
 </file>
@@ -123,6 +126,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Thread vs Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1010,6 +1038,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Thread vs Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3377,10 +3430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C556BF45-DDDD-5B49-A9B0-E46566E4D088}">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3517,7 +3570,7 @@
         <v>4.8267220000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3525,7 +3578,7 @@
         <v>4.8971150000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3533,7 +3586,7 @@
         <v>4.7430089999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3541,7 +3594,7 @@
         <v>4.7050020000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3549,7 +3602,7 @@
         <v>4.8196479999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3557,7 +3610,7 @@
         <v>4.875934</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3565,7 +3618,7 @@
         <v>4.6892149999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3573,7 +3626,7 @@
         <v>4.7348809999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3581,7 +3634,7 @@
         <v>4.7236919999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3589,7 +3642,7 @@
         <v>4.6868499999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3597,7 +3650,7 @@
         <v>4.8358759999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3605,15 +3658,22 @@
         <v>4.7373060000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
         <v>5.0382189999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <f>MIN(B:B)</f>
+        <v>3.0769030000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3621,7 +3681,7 @@
         <v>5.091107</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3629,7 +3689,7 @@
         <v>4.8791450000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3637,7 +3697,7 @@
         <v>4.7440429999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4197,10 +4257,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5E8B66-0232-A345-AF80-BB3C0C9C4BB6}">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4465,7 +4525,7 @@
         <v>3.240707</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4473,15 +4533,22 @@
         <v>3.3042729999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
         <v>3.2519</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <f>MIN(B:B)</f>
+        <v>0.37077399999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4489,7 +4556,7 @@
         <v>3.2117010000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4497,7 +4564,7 @@
         <v>3.0231979999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4505,7 +4572,7 @@
         <v>3.2836029999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4513,7 +4580,7 @@
         <v>3.251007</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4521,7 +4588,7 @@
         <v>3.2897020000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4529,7 +4596,7 @@
         <v>3.2773720000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4537,7 +4604,7 @@
         <v>3.2843179999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4545,7 +4612,7 @@
         <v>3.29528</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4553,7 +4620,7 @@
         <v>3.20384</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4561,7 +4628,7 @@
         <v>3.1930869999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4569,7 +4636,7 @@
         <v>3.2064910000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4577,7 +4644,7 @@
         <v>3.2415959999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4585,7 +4652,7 @@
         <v>3.313536</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5011,6 +5078,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>